<commit_message>
fixes on excel export, implemented export of registry of trainers
</commit_message>
<xml_diff>
--- a/quality/src/main/resources/feedback_results_report.xlsx
+++ b/quality/src/main/resources/feedback_results_report.xlsx
@@ -124,7 +124,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -169,12 +169,6 @@
       <name val="Century Gothic"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -256,7 +250,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,31 +271,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -341,7 +331,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.70703125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -349,13 +339,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="1" width="3.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.43"/>
@@ -442,10 +431,10 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="O7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -456,113 +445,113 @@
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="11" s="12" customFormat="true" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+    </row>
+    <row r="11" s="11" customFormat="true" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="10" t="s">
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="O11" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="20">

</xml_diff>